<commit_message>
Stage at DAM corrected
</commit_message>
<xml_diff>
--- a/Data/Q/LBJ_cross_section.xlsx
+++ b/Data/Q/LBJ_cross_section.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="LBJ" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="R2_m" sheetId="4" r:id="rId4"/>
     <sheet name="DAM" sheetId="6" r:id="rId5"/>
     <sheet name="DAM_m" sheetId="7" r:id="rId6"/>
+    <sheet name="DAM_m (2)" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="24">
   <si>
     <t>LBJ Bridge Cross Section</t>
   </si>
@@ -219,7 +220,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -570,11 +581,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218764784"/>
-        <c:axId val="218769096"/>
+        <c:axId val="376614008"/>
+        <c:axId val="376623024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218764784"/>
+        <c:axId val="376614008"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="16"/>
@@ -611,12 +622,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="218769096"/>
+        <c:crossAx val="376623024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218769096"/>
+        <c:axId val="376623024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -645,7 +656,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="218764784"/>
+        <c:crossAx val="376614008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -746,10 +757,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>DAM_m!$F$7:$F$40</c:f>
+              <c:f>DAM_m!$F$7:$F$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>0.30480000000000002</c:v>
                 </c:pt>
@@ -757,99 +768,69 @@
                   <c:v>0.60960000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.91439999999999999</c:v>
+                  <c:v>1.2192000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2192000000000001</c:v>
+                  <c:v>1.8288</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.524</c:v>
+                  <c:v>2.4384000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8288</c:v>
+                  <c:v>3.048</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.1336000000000004</c:v>
+                  <c:v>3.6576</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.4384000000000001</c:v>
+                  <c:v>4.2672000000000008</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.7431999999999999</c:v>
+                  <c:v>4.5720000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.048</c:v>
+                  <c:v>4.5720000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.3528000000000002</c:v>
+                  <c:v>5.4863999999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.6576</c:v>
+                  <c:v>6.0960000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.9624000000000001</c:v>
+                  <c:v>6.7056000000000004</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.2672000000000008</c:v>
+                  <c:v>7.62</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.5720000000000001</c:v>
+                  <c:v>7.62</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.5720000000000001</c:v>
+                  <c:v>7.9248000000000003</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.1815999999999995</c:v>
+                  <c:v>8.2296000000000014</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.4863999999999997</c:v>
+                  <c:v>8.5344000000000015</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.7911999999999999</c:v>
+                  <c:v>8.8391999999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.0960000000000001</c:v>
+                  <c:v>9.1440000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.4008000000000003</c:v>
+                  <c:v>9.4488000000000003</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6.7056000000000004</c:v>
+                  <c:v>9.7536000000000005</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.0103999999999997</c:v>
+                  <c:v>10.058400000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.62</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>7.62</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>7.9248000000000003</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>8.2296000000000014</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>8.5344000000000015</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>8.8391999999999999</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>9.1440000000000001</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>9.4488000000000003</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>9.7536000000000005</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>10.058400000000001</c:v>
-                </c:pt>
-                <c:pt idx="33">
                   <c:v>10.058400000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -857,80 +838,80 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>DAM_m!$H$7:$H$40</c:f>
+              <c:f>DAM_m!$H$7:$H$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>-0.3175</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-0.40640000000000004</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.55880000000000007</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.55880000000000007</c:v>
+                  <c:v>-0.70484999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.90170000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.70484999999999998</c:v>
+                  <c:v>-1.0287000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.2001500000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.90170000000000006</c:v>
+                  <c:v>-1.3525499999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.4097</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.0287000000000002</c:v>
+                  <c:v>-1.8605500000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.8605500000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-1.2001500000000001</c:v>
+                  <c:v>-1.8669</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.8669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-1.3525499999999999</c:v>
+                  <c:v>-1.8605500000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-1.4097</c:v>
+                  <c:v>-1.4224000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1.8605500000000001</c:v>
+                  <c:v>-1.3334999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.27</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-1.8605500000000001</c:v>
+                  <c:v>-1.1684000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-1.016</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-1.8669</c:v>
+                  <c:v>-0.99695000000000011</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.95250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-1.8669</c:v>
+                  <c:v>-0.85724999999999996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.82550000000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-1.8605500000000001</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-1.4224000000000001</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-1.3334999999999999</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>-1.27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-1.1684000000000001</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-1.016</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>-0.99695000000000011</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>-0.95250000000000001</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>-0.85724999999999996</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>-0.82550000000000001</c:v>
-                </c:pt>
-                <c:pt idx="33">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -946,11 +927,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="418621768"/>
-        <c:axId val="418618240"/>
+        <c:axId val="376612832"/>
+        <c:axId val="376617144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="418621768"/>
+        <c:axId val="376612832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-1"/>
@@ -1008,12 +989,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418618240"/>
+        <c:crossAx val="376617144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="418618240"/>
+        <c:axId val="376617144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1070,7 +1051,460 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418621768"/>
+        <c:crossAx val="376612832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'DAM_m (2)'!$F$7:$F$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0.30480000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.60960000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91439999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2192000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.524</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8288</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1336000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4384000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.7431999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.048</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3528000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.6576</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.9624000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.2672000000000008</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.5720000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.5720000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.1815999999999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.4863999999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.7911999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.0960000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.4008000000000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.7056000000000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.0103999999999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.62</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.62</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.9248000000000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.2296000000000014</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.5344000000000015</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.8391999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9.1440000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9.4488000000000003</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.7536000000000005</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10.058400000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10.058400000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'DAM_m (2)'!$H$7:$H$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>-0.3175</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.40640000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.55880000000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.70484999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.90170000000000006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1.0287000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.2001500000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.3525499999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.4097</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.8605500000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1.8605500000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-1.8669</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-1.8669</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-1.8605500000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-1.4224000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-1.3334999999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-1.27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-1.1684000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-1.016</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.99695000000000011</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.95250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.85724999999999996</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.82550000000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="369374496"/>
+        <c:axId val="369373320"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="369374496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="-1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="369373320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="369373320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="369374496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1350,11 +1784,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218766352"/>
-        <c:axId val="218766744"/>
+        <c:axId val="376620280"/>
+        <c:axId val="376618712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218766352"/>
+        <c:axId val="376620280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-1"/>
@@ -1412,12 +1846,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218766744"/>
+        <c:crossAx val="376618712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218766744"/>
+        <c:axId val="376618712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1474,7 +1908,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218766352"/>
+        <c:crossAx val="376620280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1538,6 +1972,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1792,11 +2227,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218758904"/>
-        <c:axId val="218770272"/>
+        <c:axId val="376615968"/>
+        <c:axId val="376621456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218758904"/>
+        <c:axId val="376615968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1839,13 +2274,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218770272"/>
+        <c:crossAx val="376621456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218770272"/>
+        <c:axId val="376621456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1896,7 +2331,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218758904"/>
+        <c:crossAx val="376615968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2128,11 +2563,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218758512"/>
-        <c:axId val="538899944"/>
+        <c:axId val="376614400"/>
+        <c:axId val="376613616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218758512"/>
+        <c:axId val="376614400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-1"/>
@@ -2190,12 +2625,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="538899944"/>
+        <c:crossAx val="376613616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="538899944"/>
+        <c:axId val="376613616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2252,7 +2687,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218758512"/>
+        <c:crossAx val="376614400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2316,7 +2751,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2523,11 +2957,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="538909744"/>
-        <c:axId val="538902296"/>
+        <c:axId val="376611264"/>
+        <c:axId val="376622632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="538909744"/>
+        <c:axId val="376611264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2570,13 +3004,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="538902296"/>
+        <c:crossAx val="376622632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="538902296"/>
+        <c:axId val="376622632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2627,7 +3061,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="538909744"/>
+        <c:crossAx val="376611264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2865,11 +3299,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="538910528"/>
-        <c:axId val="538909352"/>
+        <c:axId val="376612048"/>
+        <c:axId val="376612440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="538910528"/>
+        <c:axId val="376612048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-1"/>
@@ -2927,12 +3361,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="538909352"/>
+        <c:crossAx val="376612440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="538909352"/>
+        <c:axId val="376612440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2989,7 +3423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="538910528"/>
+        <c:crossAx val="376612048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3053,7 +3487,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3263,11 +3696,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="538904256"/>
-        <c:axId val="538898768"/>
+        <c:axId val="376614792"/>
+        <c:axId val="376615184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="538904256"/>
+        <c:axId val="376614792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3310,13 +3743,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="538898768"/>
+        <c:crossAx val="376615184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="538898768"/>
+        <c:axId val="376615184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3367,7 +3800,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="538904256"/>
+        <c:crossAx val="376614792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3431,7 +3864,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3621,11 +4053,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="418615496"/>
-        <c:axId val="418603736"/>
+        <c:axId val="376616360"/>
+        <c:axId val="376616752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="418615496"/>
+        <c:axId val="376616360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-1"/>
@@ -3683,12 +4115,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418603736"/>
+        <c:crossAx val="376616752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="418603736"/>
+        <c:axId val="376616752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3745,7 +4177,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418615496"/>
+        <c:crossAx val="376616360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4070,11 +4502,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="418608832"/>
-        <c:axId val="418607656"/>
+        <c:axId val="376618320"/>
+        <c:axId val="376622240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="418608832"/>
+        <c:axId val="376618320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4117,13 +4549,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418607656"/>
+        <c:crossAx val="376622240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="418607656"/>
+        <c:axId val="376622240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4174,7 +4606,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418608832"/>
+        <c:crossAx val="376618320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4224,6 +4656,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5099,6 +5571,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -9488,6 +10476,43 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>204787</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>509587</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>138112</xdr:colOff>
       <xdr:row>32</xdr:row>
@@ -10362,7 +11387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -11585,7 +12610,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L6:M26">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12475,7 +13500,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L6:M26">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13432,7 +14457,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L7:M27">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13607,7 +14632,7 @@
         <v>-31.75</v>
       </c>
       <c r="I7" s="12">
-        <f t="shared" ref="I7:I40" si="0">H7+MAX($G$7:$G$27)</f>
+        <f t="shared" ref="I7:I39" si="0">H7+MAX($G$7:$G$27)</f>
         <v>154.94</v>
       </c>
       <c r="J7">
@@ -15278,7 +16303,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L7:M39">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15290,9 +16315,1333 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:R30"/>
+  <sheetViews>
+    <sheetView topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>41390</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1015</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4">
+        <v>0.02</v>
+      </c>
+      <c r="O4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5">
+        <f>SUM(N16:N29)</f>
+        <v>-30.418963799999997</v>
+      </c>
+      <c r="P5" t="e">
+        <f>#REF!*AVERAGE(I8:I18)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5">
+        <f>SUM(Q7:Q18)</f>
+        <v>40.022380722069485</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="7">
+        <f>DAM!F6*0.01</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
+        <f>DAM!G6*0.01</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="10">
+        <f>DAM!H6*0.01</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="19"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7">
+        <f>DAM!F7*0.01</f>
+        <v>0.30480000000000002</v>
+      </c>
+      <c r="G7" s="10">
+        <f>DAM!G7*0.01</f>
+        <v>0.3175</v>
+      </c>
+      <c r="H7" s="10">
+        <f>DAM!H7*0.01</f>
+        <v>-0.3175</v>
+      </c>
+      <c r="I7" s="12">
+        <f>H7+MAX($G$7:$G$18)</f>
+        <v>1.5493999999999999</v>
+      </c>
+      <c r="J7">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="12">
+        <f t="shared" ref="K7:K29" si="0">F7-J7</f>
+        <v>0.30480000000000002</v>
+      </c>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12">
+        <f>$L$4-I7</f>
+        <v>-1.5293999999999999</v>
+      </c>
+      <c r="N7">
+        <f>K7*(L7+M7)*0.5</f>
+        <v>-0.23308055999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="7">
+        <f>B7+1</f>
+        <v>2</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>4</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7">
+        <f>DAM!F8*0.01</f>
+        <v>0.60960000000000003</v>
+      </c>
+      <c r="G8" s="10">
+        <f>DAM!G8*0.01</f>
+        <v>0.40640000000000004</v>
+      </c>
+      <c r="H8" s="10">
+        <f>DAM!H8*0.01</f>
+        <v>-0.40640000000000004</v>
+      </c>
+      <c r="I8" s="12">
+        <f t="shared" ref="I8:I29" si="1">H8+MAX($G$7:$G$18)</f>
+        <v>1.4604999999999999</v>
+      </c>
+      <c r="J8">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <f t="shared" ref="K8:K29" si="2">F8-J8</f>
+        <v>0.60960000000000003</v>
+      </c>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12">
+        <f t="shared" ref="M8:M29" si="3">$L$4-I8</f>
+        <v>-1.4404999999999999</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ref="N8:N29" si="4">K8*(L8+M8)*0.5</f>
+        <v>-0.43906439999999997</v>
+      </c>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12">
+        <f>SQRT(K8^2+M8^2)</f>
+        <v>1.5641778703203801</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7">
+        <f>DAM!F10*0.01</f>
+        <v>1.2192000000000001</v>
+      </c>
+      <c r="G9" s="10">
+        <f>DAM!G10*0.01</f>
+        <v>0.55880000000000007</v>
+      </c>
+      <c r="H9" s="10">
+        <f>DAM!H10*0.01</f>
+        <v>-0.55880000000000007</v>
+      </c>
+      <c r="I9" s="12">
+        <f t="shared" si="1"/>
+        <v>1.3081</v>
+      </c>
+      <c r="J9">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="12">
+        <f t="shared" si="2"/>
+        <v>1.2192000000000001</v>
+      </c>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12">
+        <f t="shared" si="3"/>
+        <v>-1.2881</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>-0.78522576000000011</v>
+      </c>
+      <c r="Q9" s="12">
+        <f t="shared" ref="Q9:Q29" si="5">SQRT(K9^2+M9^2)</f>
+        <v>1.7735981083661541</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C10" s="7">
+        <v>2</v>
+      </c>
+      <c r="D10" s="7">
+        <v>3.75</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7">
+        <f>DAM!F12*0.01</f>
+        <v>1.8288</v>
+      </c>
+      <c r="G10" s="10">
+        <f>DAM!G12*0.01</f>
+        <v>0.70484999999999998</v>
+      </c>
+      <c r="H10" s="10">
+        <f>DAM!H12*0.01</f>
+        <v>-0.70484999999999998</v>
+      </c>
+      <c r="I10" s="12">
+        <f t="shared" si="1"/>
+        <v>1.16205</v>
+      </c>
+      <c r="J10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="12">
+        <f t="shared" si="2"/>
+        <v>1.8288</v>
+      </c>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12">
+        <f t="shared" si="3"/>
+        <v>-1.14205</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>-1.0442905199999999</v>
+      </c>
+      <c r="Q10" s="12">
+        <f t="shared" si="5"/>
+        <v>2.1561047382954288</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C11" s="7">
+        <v>2</v>
+      </c>
+      <c r="D11" s="7">
+        <v>11.5</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7">
+        <f>DAM!F14*0.01</f>
+        <v>2.4384000000000001</v>
+      </c>
+      <c r="G11" s="10">
+        <f>DAM!G14*0.01</f>
+        <v>0.90170000000000006</v>
+      </c>
+      <c r="H11" s="10">
+        <f>DAM!H14*0.01</f>
+        <v>-0.90170000000000006</v>
+      </c>
+      <c r="I11" s="12">
+        <f t="shared" si="1"/>
+        <v>0.96519999999999995</v>
+      </c>
+      <c r="J11">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="12">
+        <f t="shared" si="2"/>
+        <v>2.4384000000000001</v>
+      </c>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12">
+        <f t="shared" si="3"/>
+        <v>-0.94519999999999993</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>-1.1523878400000001</v>
+      </c>
+      <c r="Q11" s="12">
+        <f t="shared" si="5"/>
+        <v>2.6151859589711779</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C12" s="7">
+        <v>3</v>
+      </c>
+      <c r="D12" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7">
+        <f>DAM!F16*0.01</f>
+        <v>3.048</v>
+      </c>
+      <c r="G12" s="10">
+        <f>DAM!G16*0.01</f>
+        <v>1.0287000000000002</v>
+      </c>
+      <c r="H12" s="10">
+        <f>DAM!H16*0.01</f>
+        <v>-1.0287000000000002</v>
+      </c>
+      <c r="I12" s="12">
+        <f t="shared" si="1"/>
+        <v>0.83819999999999983</v>
+      </c>
+      <c r="J12">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="12">
+        <f t="shared" si="2"/>
+        <v>3.048</v>
+      </c>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12">
+        <f t="shared" si="3"/>
+        <v>-0.81819999999999982</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>-1.2469367999999998</v>
+      </c>
+      <c r="Q12" s="12">
+        <f t="shared" si="5"/>
+        <v>3.1559079897867743</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C13" s="7">
+        <v>3</v>
+      </c>
+      <c r="D13" s="7">
+        <v>11.25</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7">
+        <f>DAM!F18*0.01</f>
+        <v>3.6576</v>
+      </c>
+      <c r="G13" s="10">
+        <f>DAM!G18*0.01</f>
+        <v>1.2001500000000001</v>
+      </c>
+      <c r="H13" s="10">
+        <f>DAM!H18*0.01</f>
+        <v>-1.2001500000000001</v>
+      </c>
+      <c r="I13" s="12">
+        <f t="shared" si="1"/>
+        <v>0.66674999999999995</v>
+      </c>
+      <c r="J13">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="12">
+        <f t="shared" si="2"/>
+        <v>3.6576</v>
+      </c>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12">
+        <f t="shared" si="3"/>
+        <v>-0.64674999999999994</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>-1.1827763999999998</v>
+      </c>
+      <c r="Q13" s="12">
+        <f t="shared" si="5"/>
+        <v>3.7143402270793664</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C14" s="7">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7">
+        <v>5.25</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7">
+        <f>DAM!F20*0.01</f>
+        <v>4.2672000000000008</v>
+      </c>
+      <c r="G14" s="10">
+        <f>DAM!G20*0.01</f>
+        <v>1.3525499999999999</v>
+      </c>
+      <c r="H14" s="10">
+        <f>DAM!H20*0.01</f>
+        <v>-1.3525499999999999</v>
+      </c>
+      <c r="I14" s="12">
+        <f t="shared" si="1"/>
+        <v>0.51435000000000008</v>
+      </c>
+      <c r="J14">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="12">
+        <f t="shared" si="2"/>
+        <v>4.2672000000000008</v>
+      </c>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12">
+        <f t="shared" si="3"/>
+        <v>-0.49435000000000007</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="4"/>
+        <v>-1.0547451600000004</v>
+      </c>
+      <c r="Q14" s="12">
+        <f t="shared" si="5"/>
+        <v>4.2957394895989687</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="e">
+        <f t="shared" ref="B15:B29" si="6">B14+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C15" s="7">
+        <v>4</v>
+      </c>
+      <c r="D15" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7">
+        <f>DAM!F21*0.01</f>
+        <v>4.5720000000000001</v>
+      </c>
+      <c r="G15" s="10">
+        <f>DAM!G21*0.01</f>
+        <v>1.4097</v>
+      </c>
+      <c r="H15" s="10">
+        <f>DAM!H21*0.01</f>
+        <v>-1.4097</v>
+      </c>
+      <c r="I15" s="12">
+        <f t="shared" si="1"/>
+        <v>0.45720000000000005</v>
+      </c>
+      <c r="J15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="12">
+        <f t="shared" si="2"/>
+        <v>4.5720000000000001</v>
+      </c>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12">
+        <f t="shared" si="3"/>
+        <v>-0.43720000000000003</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="4"/>
+        <v>-0.99943920000000008</v>
+      </c>
+      <c r="Q15" s="12">
+        <f t="shared" si="5"/>
+        <v>4.5928561745388894</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C16" s="7">
+        <v>6</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7">
+        <f>F15</f>
+        <v>4.5720000000000001</v>
+      </c>
+      <c r="G16" s="10">
+        <f>DAM!G22*0.01</f>
+        <v>1.8605500000000001</v>
+      </c>
+      <c r="H16" s="10">
+        <f>DAM!H22*0.01</f>
+        <v>-1.8605500000000001</v>
+      </c>
+      <c r="I16" s="12">
+        <f t="shared" si="1"/>
+        <v>6.3499999999998558E-3</v>
+      </c>
+      <c r="J16">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="12">
+        <f t="shared" si="2"/>
+        <v>4.5720000000000001</v>
+      </c>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12">
+        <f t="shared" si="3"/>
+        <v>1.3650000000000145E-2</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="4"/>
+        <v>3.1203900000000333E-2</v>
+      </c>
+      <c r="Q16" s="12">
+        <f t="shared" si="5"/>
+        <v>4.572020376430971</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="7" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C17" s="7">
+        <v>6</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7">
+        <f>DAM!F24*0.01</f>
+        <v>5.4863999999999997</v>
+      </c>
+      <c r="G17" s="10">
+        <f>DAM!G24*0.01</f>
+        <v>1.8605500000000001</v>
+      </c>
+      <c r="H17" s="10">
+        <f>DAM!H24*0.01</f>
+        <v>-1.8605500000000001</v>
+      </c>
+      <c r="I17" s="12">
+        <f t="shared" si="1"/>
+        <v>6.3499999999998558E-3</v>
+      </c>
+      <c r="J17">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="12">
+        <f t="shared" si="2"/>
+        <v>5.4863999999999997</v>
+      </c>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12">
+        <f t="shared" si="3"/>
+        <v>1.3650000000000145E-2</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="4"/>
+        <v>3.7444680000000397E-2</v>
+      </c>
+      <c r="Q17" s="12">
+        <f t="shared" si="5"/>
+        <v>5.4864169803707039</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="7" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C18" s="7">
+        <v>6</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7">
+        <f>DAM!F26*0.01</f>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="G18" s="10">
+        <f>DAM!G26*0.01</f>
+        <v>1.8669</v>
+      </c>
+      <c r="H18" s="10">
+        <f>DAM!H26*0.01</f>
+        <v>-1.8669</v>
+      </c>
+      <c r="I18" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="12">
+        <f t="shared" si="2"/>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="4"/>
+        <v>6.096E-2</v>
+      </c>
+      <c r="Q18" s="12">
+        <f t="shared" si="5"/>
+        <v>6.0960328083106639</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C19" s="7">
+        <v>6</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7">
+        <f>DAM!F28*0.01</f>
+        <v>6.7056000000000004</v>
+      </c>
+      <c r="G19" s="10">
+        <f>DAM!G28*0.01</f>
+        <v>1.8669</v>
+      </c>
+      <c r="H19" s="10">
+        <f>DAM!H28*0.01</f>
+        <v>-1.8669</v>
+      </c>
+      <c r="I19" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="12">
+        <f t="shared" si="2"/>
+        <v>6.7056000000000004</v>
+      </c>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="4"/>
+        <v>6.7056000000000004E-2</v>
+      </c>
+      <c r="Q19" s="12">
+        <f t="shared" si="5"/>
+        <v>6.7056298257508971</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C20" s="7">
+        <v>6</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7">
+        <f>F21</f>
+        <v>7.62</v>
+      </c>
+      <c r="G20" s="10">
+        <f>DAM!G30*0.01</f>
+        <v>1.8605500000000001</v>
+      </c>
+      <c r="H20" s="10">
+        <f>DAM!H30*0.01</f>
+        <v>-1.8605500000000001</v>
+      </c>
+      <c r="I20" s="12">
+        <f t="shared" si="1"/>
+        <v>6.3499999999998558E-3</v>
+      </c>
+      <c r="J20">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="12">
+        <f t="shared" si="2"/>
+        <v>7.62</v>
+      </c>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12">
+        <f t="shared" si="3"/>
+        <v>1.3650000000000145E-2</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="4"/>
+        <v>5.2006500000000552E-2</v>
+      </c>
+      <c r="Q20" s="12">
+        <f t="shared" si="5"/>
+        <v>7.6200122258760192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C21" s="7">
+        <v>4</v>
+      </c>
+      <c r="D21" s="7">
+        <v>8</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7">
+        <f>DAM!F31*0.01</f>
+        <v>7.62</v>
+      </c>
+      <c r="G21" s="10">
+        <f>DAM!G31*0.01</f>
+        <v>1.4224000000000001</v>
+      </c>
+      <c r="H21" s="10">
+        <f>DAM!H31*0.01</f>
+        <v>-1.4224000000000001</v>
+      </c>
+      <c r="I21" s="12">
+        <f t="shared" si="1"/>
+        <v>0.4444999999999999</v>
+      </c>
+      <c r="J21">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="12">
+        <f t="shared" si="2"/>
+        <v>7.62</v>
+      </c>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12">
+        <f t="shared" si="3"/>
+        <v>-0.42449999999999988</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="4"/>
+        <v>-1.6173449999999996</v>
+      </c>
+      <c r="Q21" s="12">
+        <f t="shared" si="5"/>
+        <v>7.6318150036541113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C22" s="7">
+        <v>4</v>
+      </c>
+      <c r="D22" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7">
+        <f>DAM!F32*0.01</f>
+        <v>7.9248000000000003</v>
+      </c>
+      <c r="G22" s="10">
+        <f>DAM!G32*0.01</f>
+        <v>1.3334999999999999</v>
+      </c>
+      <c r="H22" s="10">
+        <f>DAM!H32*0.01</f>
+        <v>-1.3334999999999999</v>
+      </c>
+      <c r="I22" s="12">
+        <f t="shared" si="1"/>
+        <v>0.5334000000000001</v>
+      </c>
+      <c r="J22">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="12">
+        <f t="shared" si="2"/>
+        <v>7.9248000000000003</v>
+      </c>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12">
+        <f t="shared" si="3"/>
+        <v>-0.51340000000000008</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="4"/>
+        <v>-2.0342961600000002</v>
+      </c>
+      <c r="Q22" s="12">
+        <f t="shared" si="5"/>
+        <v>7.9414126325232592</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C23" s="7">
+        <v>4</v>
+      </c>
+      <c r="D23" s="7">
+        <v>2</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7">
+        <f>DAM!F33*0.01</f>
+        <v>8.2296000000000014</v>
+      </c>
+      <c r="G23" s="10">
+        <f>DAM!G33*0.01</f>
+        <v>1.27</v>
+      </c>
+      <c r="H23" s="10">
+        <f>DAM!H33*0.01</f>
+        <v>-1.27</v>
+      </c>
+      <c r="I23" s="12">
+        <f t="shared" si="1"/>
+        <v>0.59689999999999999</v>
+      </c>
+      <c r="J23">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K23" s="12">
+        <f t="shared" si="2"/>
+        <v>8.2296000000000014</v>
+      </c>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12">
+        <f t="shared" si="3"/>
+        <v>-0.57689999999999997</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="4"/>
+        <v>-2.3738281200000002</v>
+      </c>
+      <c r="Q23" s="12">
+        <f t="shared" si="5"/>
+        <v>8.2497957411077785</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C24" s="7">
+        <v>3</v>
+      </c>
+      <c r="D24" s="7">
+        <v>10</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7">
+        <f>DAM!F34*0.01</f>
+        <v>8.5344000000000015</v>
+      </c>
+      <c r="G24" s="10">
+        <f>DAM!G34*0.01</f>
+        <v>1.1684000000000001</v>
+      </c>
+      <c r="H24" s="10">
+        <f>DAM!H34*0.01</f>
+        <v>-1.1684000000000001</v>
+      </c>
+      <c r="I24" s="12">
+        <f t="shared" si="1"/>
+        <v>0.6984999999999999</v>
+      </c>
+      <c r="J24">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="12">
+        <f t="shared" si="2"/>
+        <v>8.5344000000000015</v>
+      </c>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12">
+        <f t="shared" si="3"/>
+        <v>-0.67849999999999988</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="4"/>
+        <v>-2.8952952000000001</v>
+      </c>
+      <c r="Q24" s="12">
+        <f t="shared" si="5"/>
+        <v>8.5613284956249647</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C25" s="7">
+        <v>3</v>
+      </c>
+      <c r="D25" s="7">
+        <v>4</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7">
+        <f>DAM!F35*0.01</f>
+        <v>8.8391999999999999</v>
+      </c>
+      <c r="G25" s="10">
+        <f>DAM!G35*0.01</f>
+        <v>1.016</v>
+      </c>
+      <c r="H25" s="10">
+        <f>DAM!H35*0.01</f>
+        <v>-1.016</v>
+      </c>
+      <c r="I25" s="12">
+        <f t="shared" si="1"/>
+        <v>0.85089999999999999</v>
+      </c>
+      <c r="J25">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="12">
+        <f t="shared" si="2"/>
+        <v>8.8391999999999999</v>
+      </c>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12">
+        <f t="shared" si="3"/>
+        <v>-0.83089999999999997</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="4"/>
+        <v>-3.6722456399999999</v>
+      </c>
+      <c r="Q25" s="12">
+        <f t="shared" si="5"/>
+        <v>8.878167122216162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C26" s="7">
+        <v>3</v>
+      </c>
+      <c r="D26" s="7">
+        <v>3.25</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7">
+        <f>DAM!F36*0.01</f>
+        <v>9.1440000000000001</v>
+      </c>
+      <c r="G26" s="10">
+        <f>DAM!G36*0.01</f>
+        <v>0.99695000000000011</v>
+      </c>
+      <c r="H26" s="10">
+        <f>DAM!H36*0.01</f>
+        <v>-0.99695000000000011</v>
+      </c>
+      <c r="I26" s="12">
+        <f t="shared" si="1"/>
+        <v>0.86994999999999989</v>
+      </c>
+      <c r="J26">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="12">
+        <f t="shared" si="2"/>
+        <v>9.1440000000000001</v>
+      </c>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12">
+        <f t="shared" si="3"/>
+        <v>-0.84994999999999987</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="4"/>
+        <v>-3.8859713999999994</v>
+      </c>
+      <c r="Q26" s="12">
+        <f t="shared" si="5"/>
+        <v>9.1834171745870279</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="e">
+        <f>B26+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C27" s="7">
+        <v>3</v>
+      </c>
+      <c r="D27" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7">
+        <f>DAM!F37*0.01</f>
+        <v>9.4488000000000003</v>
+      </c>
+      <c r="G27" s="10">
+        <f>DAM!G37*0.01</f>
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="H27" s="10">
+        <f>DAM!H37*0.01</f>
+        <v>-0.95250000000000001</v>
+      </c>
+      <c r="I27" s="12">
+        <f t="shared" si="1"/>
+        <v>0.91439999999999999</v>
+      </c>
+      <c r="J27">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="12">
+        <f t="shared" si="2"/>
+        <v>9.4488000000000003</v>
+      </c>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12">
+        <f t="shared" si="3"/>
+        <v>-0.89439999999999997</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="4"/>
+        <v>-4.2255033600000003</v>
+      </c>
+      <c r="Q27" s="12">
+        <f t="shared" si="5"/>
+        <v>9.4910364449832354</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C28" s="7">
+        <v>2</v>
+      </c>
+      <c r="D28" s="7">
+        <v>9.75</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7">
+        <f>DAM!F38*0.01</f>
+        <v>9.7536000000000005</v>
+      </c>
+      <c r="G28" s="10">
+        <f>DAM!G38*0.01</f>
+        <v>0.85724999999999996</v>
+      </c>
+      <c r="H28" s="10">
+        <f>DAM!H38*0.01</f>
+        <v>-0.85724999999999996</v>
+      </c>
+      <c r="I28" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0096500000000002</v>
+      </c>
+      <c r="J28">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="12">
+        <f t="shared" si="2"/>
+        <v>9.7536000000000005</v>
+      </c>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12">
+        <f t="shared" si="3"/>
+        <v>-0.98965000000000014</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="4"/>
+        <v>-4.8263251200000008</v>
+      </c>
+      <c r="Q28" s="12">
+        <f t="shared" si="5"/>
+        <v>9.8036789055180709</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C29" s="7">
+        <v>2</v>
+      </c>
+      <c r="D29" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7">
+        <f>DAM!F39*0.01</f>
+        <v>10.058400000000001</v>
+      </c>
+      <c r="G29" s="10">
+        <f>DAM!G39*0.01</f>
+        <v>0.82550000000000001</v>
+      </c>
+      <c r="H29" s="10">
+        <f>DAM!H39*0.01</f>
+        <v>-0.82550000000000001</v>
+      </c>
+      <c r="I29" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0413999999999999</v>
+      </c>
+      <c r="J29">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="12">
+        <f t="shared" si="2"/>
+        <v>10.058400000000001</v>
+      </c>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12">
+        <f t="shared" si="3"/>
+        <v>-1.0213999999999999</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="4"/>
+        <v>-5.1368248799999998</v>
+      </c>
+      <c r="Q29" s="12">
+        <f t="shared" si="5"/>
+        <v>10.110127027886445</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>33</v>
+      </c>
+      <c r="F30" s="7">
+        <f>DAM!F40*0.01</f>
+        <v>10.058400000000001</v>
+      </c>
+      <c r="G30" s="10">
+        <f>DAM!G40*0.01</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="10">
+        <f>DAM!H40*0.01</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="L7:M29">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -17098,7 +19447,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L7:M39">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>